<commit_message>
recovered hopefully all code
</commit_message>
<xml_diff>
--- a/plate_files/drugs.xlsx
+++ b/plate_files/drugs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malte/Documents/global_scripts/pypetting_experiments/CombinationExperiment/plate_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8E954C-EB85-914C-9D86-6E2C4155DE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CC24E9-D0C0-9144-A5C2-6CE2EAC6691F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="680" windowWidth="35840" windowHeight="21900" xr2:uid="{F79A83FD-92F4-C049-9C19-433DFCCE3398}"/>
   </bookViews>
@@ -489,12 +489,13 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -528,7 +529,7 @@
         <v>17</v>
       </c>
       <c r="D2">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E2" s="1">
         <v>8</v>
@@ -548,7 +549,7 @@
         <v>18</v>
       </c>
       <c r="D3">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1">
         <v>8</v>
@@ -608,7 +609,7 @@
         <v>21</v>
       </c>
       <c r="D6">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
@@ -628,7 +629,7 @@
         <v>22</v>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
updated reservoir generation to now create the combi plates only containing drug B and an A_subreservoir
</commit_message>
<xml_diff>
--- a/plate_files/drugs.xlsx
+++ b/plate_files/drugs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malte/Documents/global_scripts/pypetting_experiments/CombinationExperiment/plate_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CC24E9-D0C0-9144-A5C2-6CE2EAC6691F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412D70C2-2634-4A41-9ABB-94051A2DC454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="680" windowWidth="35840" windowHeight="21900" xr2:uid="{F79A83FD-92F4-C049-9C19-433DFCCE3398}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>drug</t>
   </si>
@@ -86,9 +86,6 @@
     <t>stock</t>
   </si>
   <si>
-    <t>micRef</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -114,6 +111,12 @@
   </si>
   <si>
     <t>Water</t>
+  </si>
+  <si>
+    <t>cRef</t>
+  </si>
+  <si>
+    <t>H2O</t>
   </si>
 </sst>
 </file>
@@ -489,7 +492,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -512,10 +515,10 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -526,16 +529,16 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -546,7 +549,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>32</v>
@@ -555,7 +558,7 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -566,16 +569,16 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>8</v>
       </c>
       <c r="E4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -586,16 +589,16 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5">
         <v>16</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -606,7 +609,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>16</v>
@@ -615,7 +618,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -626,7 +629,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7">
         <v>16</v>
@@ -635,7 +638,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>